<commit_message>
Forgot changes to the project file.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="117">
   <si>
     <t>Tag name</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>ParseTryElement</t>
+  </si>
+  <si>
+    <t>ParseCatchElement</t>
   </si>
 </sst>
 </file>
@@ -753,8 +756,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1176,7 @@
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated CPlusPlusCodeParser to handle SRC.<type>_decl tags.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="119">
   <si>
     <t>Tag name</t>
   </si>
@@ -363,9 +363,6 @@
     <t>ParseNamespaceElement</t>
   </si>
   <si>
-    <t>Special handling for properties</t>
-  </si>
-  <si>
     <t>ParseLabelElement</t>
   </si>
   <si>
@@ -376,6 +373,15 @@
   </si>
   <si>
     <t>ParseCatchElement</t>
+  </si>
+  <si>
+    <t>ParseForeachElement</t>
+  </si>
+  <si>
+    <t>ParseDeclarationStatementElement</t>
+  </si>
+  <si>
+    <t>Special handling for properties. Handled in ParsePropertyDeclarationElement</t>
   </si>
 </sst>
 </file>
@@ -756,8 +762,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +850,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -859,10 +865,10 @@
         <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1010,7 +1016,7 @@
         <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1135,7 +1141,7 @@
         <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1150,7 +1156,7 @@
         <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1163,7 +1169,7 @@
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1176,7 +1182,7 @@
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1189,7 +1195,7 @@
         <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,7 +1289,7 @@
         <v>73</v>
       </c>
       <c r="F35" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1312,7 +1318,7 @@
         <v>73</v>
       </c>
       <c r="F37" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,7 +1347,7 @@
         <v>73</v>
       </c>
       <c r="F39" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,7 +1376,7 @@
         <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G41" t="s">
         <v>103</v>
@@ -1389,7 +1395,7 @@
         <v>73</v>
       </c>
       <c r="F42" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G42" t="s">
         <v>103</v>
@@ -1408,7 +1414,7 @@
         <v>73</v>
       </c>
       <c r="F43" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="G43" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Implemented method parsing for C++. This is still missing parsing for the name prefix, which will be part of expression parsing.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="120">
   <si>
     <t>Tag name</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>Special handling for properties. Handled in ParsePropertyDeclarationElement</t>
+  </si>
+  <si>
+    <t>This tag doesn't actually exist?</t>
   </si>
 </sst>
 </file>
@@ -762,8 +765,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,8 +1469,8 @@
       <c r="E46" t="s">
         <v>73</v>
       </c>
-      <c r="F46" t="s">
-        <v>82</v>
+      <c r="G46" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented parsing for free-standing blocks.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="122">
   <si>
     <t>Tag name</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Finally</t>
   </si>
   <si>
-    <t>Free-standing blocks still todo. Most blocks parsed as components of e.g. IfStatements</t>
-  </si>
-  <si>
     <t>Component of IfStatement</t>
   </si>
   <si>
@@ -385,6 +382,15 @@
   </si>
   <si>
     <t>This tag doesn't actually exist?</t>
+  </si>
+  <si>
+    <t>GetParentTypeUseElements</t>
+  </si>
+  <si>
+    <t>ParseBlockElement</t>
+  </si>
+  <si>
+    <t>Free-standing blocks done by ParseBlockElement. Most blocks parsed as components of e.g. IfStatements</t>
   </si>
 </sst>
 </file>
@@ -765,8 +771,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>64</v>
@@ -820,18 +826,18 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
         <v>81</v>
       </c>
-      <c r="F3" t="s">
-        <v>82</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>70</v>
@@ -840,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -853,7 +859,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,10 +874,10 @@
         <v>77</v>
       </c>
       <c r="F6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" t="s">
         <v>117</v>
-      </c>
-      <c r="G6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -883,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,16 +901,16 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>70</v>
@@ -929,7 +935,7 @@
         <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -945,7 +951,7 @@
         <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -984,7 +990,7 @@
         <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -997,13 +1003,13 @@
         <v>26</v>
       </c>
       <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
         <v>81</v>
       </c>
-      <c r="F15" t="s">
-        <v>82</v>
-      </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1019,7 +1025,7 @@
         <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1032,7 +1038,7 @@
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,7 +1051,7 @@
         <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,7 +1064,7 @@
         <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1074,16 +1080,16 @@
         <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
         <v>70</v>
@@ -1092,7 +1098,7 @@
         <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1105,7 +1111,7 @@
         <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1118,7 +1124,7 @@
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1131,7 +1137,7 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,13 +1150,13 @@
         <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
         <v>70</v>
@@ -1159,7 +1165,7 @@
         <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,7 +1178,7 @@
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,7 +1191,7 @@
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1198,7 +1204,7 @@
         <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1210,7 +1216,7 @@
         <v>64</v>
       </c>
       <c r="F30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,10 +1228,10 @@
         <v>14</v>
       </c>
       <c r="E31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" t="s">
         <v>81</v>
-      </c>
-      <c r="F31" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1240,10 +1246,10 @@
         <v>77</v>
       </c>
       <c r="F32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1255,16 +1261,16 @@
         <v>59</v>
       </c>
       <c r="E33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" t="s">
         <v>81</v>
-      </c>
-      <c r="F33" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
@@ -1273,10 +1279,10 @@
         <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1292,7 +1298,7 @@
         <v>73</v>
       </c>
       <c r="F35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,7 +1311,7 @@
         <v>47</v>
       </c>
       <c r="F36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1321,7 +1327,7 @@
         <v>73</v>
       </c>
       <c r="F37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1334,7 +1340,7 @@
         <v>49</v>
       </c>
       <c r="F38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1350,7 +1356,7 @@
         <v>73</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1363,7 +1369,7 @@
         <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,10 +1385,10 @@
         <v>73</v>
       </c>
       <c r="F41" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" t="s">
         <v>102</v>
-      </c>
-      <c r="G41" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1398,10 +1404,10 @@
         <v>73</v>
       </c>
       <c r="F42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" t="s">
         <v>102</v>
-      </c>
-      <c r="G42" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1417,10 +1423,10 @@
         <v>73</v>
       </c>
       <c r="F43" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" t="s">
         <v>102</v>
-      </c>
-      <c r="G43" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1433,10 +1439,10 @@
         <v>57</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1449,16 +1455,16 @@
         <v>58</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>70</v>
@@ -1470,7 +1476,7 @@
         <v>73</v>
       </c>
       <c r="G46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1483,7 +1489,7 @@
         <v>39</v>
       </c>
       <c r="F47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1499,7 +1505,7 @@
         <v>73</v>
       </c>
       <c r="F48" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1512,7 +1518,7 @@
         <v>41</v>
       </c>
       <c r="F49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1525,7 +1531,7 @@
         <v>42</v>
       </c>
       <c r="F50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1538,7 +1544,7 @@
         <v>51</v>
       </c>
       <c r="F51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1554,7 +1560,7 @@
         <v>73</v>
       </c>
       <c r="F52" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1567,7 +1573,7 @@
         <v>54</v>
       </c>
       <c r="F53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1583,7 +1589,7 @@
         <v>73</v>
       </c>
       <c r="F54" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1598,7 +1604,7 @@
         <v>73</v>
       </c>
       <c r="F55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1619,7 @@
         <v>73</v>
       </c>
       <c r="F56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,7 +1634,7 @@
         <v>73</v>
       </c>
       <c r="F57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,12 +1649,12 @@
         <v>73</v>
       </c>
       <c r="F58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
@@ -1693,10 +1699,10 @@
         <v>29</v>
       </c>
       <c r="F63" t="s">
+        <v>108</v>
+      </c>
+      <c r="G63" t="s">
         <v>109</v>
-      </c>
-      <c r="G63" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1755,7 +1761,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
         <v>70</v>
@@ -1766,7 +1772,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
         <v>70</v>
@@ -1777,7 +1783,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
         <v>70</v>
@@ -1788,7 +1794,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C73" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Added parsing for extern statements
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="123">
   <si>
     <t>Tag name</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>Free-standing blocks done by ParseBlockElement. Most blocks parsed as components of e.g. IfStatements</t>
+  </si>
+  <si>
+    <t>ParseExternElement</t>
   </si>
 </sst>
 </file>
@@ -771,8 +774,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,7 +1637,7 @@
         <v>73</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added foreach parsing for Java, and updated C# version for fixes in srcML parsing.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -339,9 +339,6 @@
     <t>Need special handling for Java package statements</t>
   </si>
   <si>
-    <t>handle Java-style foreach</t>
-  </si>
-  <si>
     <t xml:space="preserve">TODO: C# override </t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>ParseExternElement</t>
+  </si>
+  <si>
+    <t>overridden in JavaCodeParser</t>
   </si>
 </sst>
 </file>
@@ -774,8 +774,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -877,10 +877,10 @@
         <v>77</v>
       </c>
       <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" t="s">
         <v>116</v>
-      </c>
-      <c r="G6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,10 +904,10 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" t="s">
         <v>120</v>
-      </c>
-      <c r="G8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1009,10 +1009,10 @@
         <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
         <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
         <v>64</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
         <v>101</v>
       </c>
       <c r="G34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>80</v>
       </c>
       <c r="F44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>73</v>
       </c>
       <c r="G46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>39</v>
       </c>
       <c r="F47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1508,7 +1508,7 @@
         <v>73</v>
       </c>
       <c r="F48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1521,7 +1521,7 @@
         <v>41</v>
       </c>
       <c r="F49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>42</v>
       </c>
       <c r="F50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>51</v>
       </c>
       <c r="F51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,7 +1563,7 @@
         <v>73</v>
       </c>
       <c r="F52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>54</v>
       </c>
       <c r="F53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>73</v>
       </c>
       <c r="F54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>73</v>
       </c>
       <c r="F57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,10 +1702,10 @@
         <v>29</v>
       </c>
       <c r="F63" t="s">
+        <v>107</v>
+      </c>
+      <c r="G63" t="s">
         <v>108</v>
-      </c>
-      <c r="G63" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added parsing for Java unit and Package elements.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -774,8 +774,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +832,7 @@
         <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>103</v>
@@ -1234,7 +1234,7 @@
         <v>80</v>
       </c>
       <c r="F31" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed ParseElement to ParseStatement. Refactored unit parsing to be called directly from ParseFileUnit.
</commit_message>
<xml_diff>
--- a/ABB.SrcML.Data/SrcMLTagParsing.xlsx
+++ b/ABB.SrcML.Data/SrcMLTagParsing.xlsx
@@ -771,11 +771,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1089,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>83</v>
@@ -1156,7 +1156,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
         <v>84</v>
@@ -1439,13 +1439,10 @@
         <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1455,7 +1452,7 @@
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
         <v>80</v>
@@ -1466,46 +1463,46 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="B46" s="4"/>
       <c r="C46" t="s">
         <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" t="s">
-        <v>117</v>
+        <v>80</v>
+      </c>
+      <c r="F46" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="C47" t="s">
         <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>39</v>
-      </c>
-      <c r="F47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" t="s">
         <v>70</v>
       </c>
       <c r="D48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E48" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F48" t="s">
         <v>105</v>
@@ -1518,7 +1515,10 @@
         <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
       </c>
       <c r="F49" t="s">
         <v>105</v>
@@ -1531,10 +1531,10 @@
         <v>70</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,10 +1544,10 @@
         <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F51" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1557,10 +1557,7 @@
         <v>70</v>
       </c>
       <c r="D52" t="s">
-        <v>53</v>
-      </c>
-      <c r="E52" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="F52" t="s">
         <v>105</v>
@@ -1573,7 +1570,10 @@
         <v>70</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="E53" t="s">
+        <v>73</v>
       </c>
       <c r="F53" t="s">
         <v>105</v>
@@ -1586,10 +1586,7 @@
         <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="F54" t="s">
         <v>105</v>
@@ -1597,17 +1594,18 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
       <c r="C55" t="s">
         <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
         <v>73</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1616,7 +1614,7 @@
         <v>70</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E56" t="s">
         <v>73</v>
@@ -1631,13 +1629,13 @@
         <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
         <v>73</v>
       </c>
       <c r="F57" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1646,33 +1644,39 @@
         <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E58" t="s">
         <v>73</v>
       </c>
       <c r="F58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C59" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="C60" t="s">
-        <v>70</v>
-      </c>
-      <c r="D60" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1681,7 +1685,7 @@
         <v>70</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,7 +1694,7 @@
         <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1699,13 +1703,7 @@
         <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>29</v>
-      </c>
-      <c r="F63" t="s">
-        <v>107</v>
-      </c>
-      <c r="G63" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,7 +1712,13 @@
         <v>70</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="F64" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1727,7 @@
         <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1732,7 +1736,7 @@
         <v>70</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,7 +1745,7 @@
         <v>70</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1750,7 +1754,7 @@
         <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,18 +1763,16 @@
         <v>70</v>
       </c>
       <c r="D69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C70" t="s">
-        <v>70</v>
-      </c>
-      <c r="D70" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,7 +1783,7 @@
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,29 +1794,29 @@
         <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>91</v>
       </c>
-      <c r="C73" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C74" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A59:A69"/>
+    <mergeCell ref="A4:A59"/>
+    <mergeCell ref="B34:B46"/>
+    <mergeCell ref="B47:B55"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B21:B25"/>
     <mergeCell ref="B9:B19"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B46:B54"/>
-    <mergeCell ref="B34:B45"/>
-    <mergeCell ref="A4:A58"/>
+    <mergeCell ref="A60:A70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>